<commit_message>
update diary entry (#257)
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -287,14 +287,27 @@
   <si>
     <t>getting to know a new tool called call graph, knowing what a senior programmer would  do when encountering problems (i.e. work together, go deep, focus on essence.)</t>
   </si>
+  <si>
+    <t>13:00 - 16:30</t>
+  </si>
+  <si>
+    <t>finish homework2</t>
+  </si>
+  <si>
+    <t>We finished team homework2, also discussed a lot about our project.</t>
+  </si>
+  <si>
+    <t>After discussing with my teammates, i know more about this project. Sometimes brainstorming brings you what u ignores before. I am learning towards the way of what a senior would do.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="60" formatCode="m/d"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -514,7 +527,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -613,6 +626,9 @@
     </xf>
     <xf numFmtId="49" fontId="15" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="13" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -2183,931 +2199,945 @@
       </c>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
+      <c r="A25" s="33">
+        <v>43866</v>
+      </c>
+      <c r="B25" t="s" s="20">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s" s="20">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s" s="27">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s" s="27">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s" s="20">
+        <v>89</v>
+      </c>
+      <c r="G25" t="s" s="32">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="33"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="33"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="35"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="35"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="33"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="33"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="33"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="35"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="33"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="33"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="33"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="33"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="33"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="33"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="33"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="33"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="33"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="33"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="33"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="33"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="33"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="33"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="33"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="33"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="33"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="33"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="33"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="33"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="33"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="33"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="33"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="35"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="33"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="35"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="33"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="35"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="33"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="35"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="33"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="35"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="33"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="35"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="33"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="35"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="33"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="35"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="33"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="35"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="33"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="35"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="33"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="34"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="35"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="33"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="35"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="33"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="35"/>
+      <c r="A80" s="34"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="33"/>
-      <c r="B81" s="34"/>
-      <c r="C81" s="34"/>
-      <c r="D81" s="34"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="35"/>
+      <c r="A81" s="34"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="33"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="34"/>
-      <c r="D82" s="34"/>
-      <c r="E82" s="34"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="35"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="33"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="35"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="33"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="35"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="33"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="35"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="35"/>
+      <c r="E85" s="35"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="33"/>
-      <c r="B86" s="34"/>
-      <c r="C86" s="34"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="35"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="33"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
-      <c r="D87" s="34"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="35"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="35"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="33"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="34"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="35"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="33"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="35"/>
+      <c r="A89" s="34"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="35"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="33"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="35"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="35"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="33"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="35"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="35"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="33"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="34"/>
-      <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="34"/>
-      <c r="G92" s="35"/>
+      <c r="A92" s="34"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="33"/>
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
-      <c r="F93" s="34"/>
-      <c r="G93" s="35"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="35"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="33"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
-      <c r="F94" s="34"/>
-      <c r="G94" s="35"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="35"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="33"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="35"/>
+      <c r="A95" s="34"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="33"/>
-      <c r="B96" s="34"/>
-      <c r="C96" s="34"/>
-      <c r="D96" s="34"/>
-      <c r="E96" s="34"/>
-      <c r="F96" s="34"/>
-      <c r="G96" s="35"/>
+      <c r="A96" s="34"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="33"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="34"/>
-      <c r="D97" s="34"/>
-      <c r="E97" s="34"/>
-      <c r="F97" s="34"/>
-      <c r="G97" s="35"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="33"/>
-      <c r="B98" s="34"/>
-      <c r="C98" s="34"/>
-      <c r="D98" s="34"/>
-      <c r="E98" s="34"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="35"/>
+      <c r="A98" s="34"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="33"/>
-      <c r="B99" s="34"/>
-      <c r="C99" s="34"/>
-      <c r="D99" s="34"/>
-      <c r="E99" s="34"/>
-      <c r="F99" s="34"/>
-      <c r="G99" s="35"/>
+      <c r="A99" s="34"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="33"/>
-      <c r="B100" s="34"/>
-      <c r="C100" s="34"/>
-      <c r="D100" s="34"/>
-      <c r="E100" s="34"/>
-      <c r="F100" s="34"/>
-      <c r="G100" s="35"/>
+      <c r="A100" s="34"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="35"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="33"/>
-      <c r="B101" s="34"/>
-      <c r="C101" s="34"/>
-      <c r="D101" s="34"/>
-      <c r="E101" s="34"/>
-      <c r="F101" s="34"/>
-      <c r="G101" s="35"/>
+      <c r="A101" s="34"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="35"/>
+      <c r="F101" s="35"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="33"/>
-      <c r="B102" s="34"/>
-      <c r="C102" s="34"/>
-      <c r="D102" s="34"/>
-      <c r="E102" s="34"/>
-      <c r="F102" s="34"/>
-      <c r="G102" s="35"/>
+      <c r="A102" s="34"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="35"/>
+      <c r="F102" s="35"/>
+      <c r="G102" s="36"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="33"/>
-      <c r="B103" s="34"/>
-      <c r="C103" s="34"/>
-      <c r="D103" s="34"/>
-      <c r="E103" s="34"/>
-      <c r="F103" s="34"/>
-      <c r="G103" s="35"/>
+      <c r="A103" s="34"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="36"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="33"/>
-      <c r="B104" s="34"/>
-      <c r="C104" s="34"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
-      <c r="F104" s="34"/>
-      <c r="G104" s="35"/>
+      <c r="A104" s="34"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="35"/>
+      <c r="F104" s="35"/>
+      <c r="G104" s="36"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="33"/>
-      <c r="B105" s="34"/>
-      <c r="C105" s="34"/>
-      <c r="D105" s="34"/>
-      <c r="E105" s="34"/>
-      <c r="F105" s="34"/>
-      <c r="G105" s="35"/>
+      <c r="A105" s="34"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
+      <c r="D105" s="35"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="35"/>
+      <c r="G105" s="36"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="33"/>
-      <c r="B106" s="34"/>
-      <c r="C106" s="34"/>
-      <c r="D106" s="34"/>
-      <c r="E106" s="34"/>
-      <c r="F106" s="34"/>
-      <c r="G106" s="35"/>
+      <c r="A106" s="34"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="35"/>
+      <c r="G106" s="36"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="33"/>
-      <c r="B107" s="34"/>
-      <c r="C107" s="34"/>
-      <c r="D107" s="34"/>
-      <c r="E107" s="34"/>
-      <c r="F107" s="34"/>
-      <c r="G107" s="35"/>
+      <c r="A107" s="34"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="35"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="33"/>
-      <c r="B108" s="34"/>
-      <c r="C108" s="34"/>
-      <c r="D108" s="34"/>
-      <c r="E108" s="34"/>
-      <c r="F108" s="34"/>
-      <c r="G108" s="35"/>
+      <c r="A108" s="34"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
+      <c r="E108" s="35"/>
+      <c r="F108" s="35"/>
+      <c r="G108" s="36"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="33"/>
-      <c r="B109" s="34"/>
-      <c r="C109" s="34"/>
-      <c r="D109" s="34"/>
-      <c r="E109" s="34"/>
-      <c r="F109" s="34"/>
-      <c r="G109" s="35"/>
+      <c r="A109" s="34"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="35"/>
+      <c r="E109" s="35"/>
+      <c r="F109" s="35"/>
+      <c r="G109" s="36"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="33"/>
-      <c r="B110" s="34"/>
-      <c r="C110" s="34"/>
-      <c r="D110" s="34"/>
-      <c r="E110" s="34"/>
-      <c r="F110" s="34"/>
-      <c r="G110" s="35"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
+      <c r="E110" s="35"/>
+      <c r="F110" s="35"/>
+      <c r="G110" s="36"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="33"/>
-      <c r="B111" s="34"/>
-      <c r="C111" s="34"/>
-      <c r="D111" s="34"/>
-      <c r="E111" s="34"/>
-      <c r="F111" s="34"/>
-      <c r="G111" s="35"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
+      <c r="E111" s="35"/>
+      <c r="F111" s="35"/>
+      <c r="G111" s="36"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="33"/>
-      <c r="B112" s="34"/>
-      <c r="C112" s="34"/>
-      <c r="D112" s="34"/>
-      <c r="E112" s="34"/>
-      <c r="F112" s="34"/>
-      <c r="G112" s="35"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
+      <c r="E112" s="35"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="33"/>
-      <c r="B113" s="34"/>
-      <c r="C113" s="34"/>
-      <c r="D113" s="34"/>
-      <c r="E113" s="34"/>
-      <c r="F113" s="34"/>
-      <c r="G113" s="35"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="35"/>
+      <c r="D113" s="35"/>
+      <c r="E113" s="35"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="36"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="33"/>
-      <c r="B114" s="34"/>
-      <c r="C114" s="34"/>
-      <c r="D114" s="34"/>
-      <c r="E114" s="34"/>
-      <c r="F114" s="34"/>
-      <c r="G114" s="35"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
+      <c r="E114" s="35"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="36"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="33"/>
-      <c r="B115" s="34"/>
-      <c r="C115" s="34"/>
-      <c r="D115" s="34"/>
-      <c r="E115" s="34"/>
-      <c r="F115" s="34"/>
-      <c r="G115" s="35"/>
+      <c r="A115" s="34"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="35"/>
+      <c r="D115" s="35"/>
+      <c r="E115" s="35"/>
+      <c r="F115" s="35"/>
+      <c r="G115" s="36"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="33"/>
-      <c r="B116" s="34"/>
-      <c r="C116" s="34"/>
-      <c r="D116" s="34"/>
-      <c r="E116" s="34"/>
-      <c r="F116" s="34"/>
-      <c r="G116" s="35"/>
+      <c r="A116" s="34"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
+      <c r="E116" s="35"/>
+      <c r="F116" s="35"/>
+      <c r="G116" s="36"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="33"/>
-      <c r="B117" s="34"/>
-      <c r="C117" s="34"/>
-      <c r="D117" s="34"/>
-      <c r="E117" s="34"/>
-      <c r="F117" s="34"/>
-      <c r="G117" s="35"/>
+      <c r="A117" s="34"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="35"/>
+      <c r="E117" s="35"/>
+      <c r="F117" s="35"/>
+      <c r="G117" s="36"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="33"/>
-      <c r="B118" s="34"/>
-      <c r="C118" s="34"/>
-      <c r="D118" s="34"/>
-      <c r="E118" s="34"/>
-      <c r="F118" s="34"/>
-      <c r="G118" s="35"/>
+      <c r="A118" s="34"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="35"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="36"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="33"/>
-      <c r="B119" s="34"/>
-      <c r="C119" s="34"/>
-      <c r="D119" s="34"/>
-      <c r="E119" s="34"/>
-      <c r="F119" s="34"/>
-      <c r="G119" s="35"/>
+      <c r="A119" s="34"/>
+      <c r="B119" s="35"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="35"/>
+      <c r="E119" s="35"/>
+      <c r="F119" s="35"/>
+      <c r="G119" s="36"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="33"/>
-      <c r="B120" s="34"/>
-      <c r="C120" s="34"/>
-      <c r="D120" s="34"/>
-      <c r="E120" s="34"/>
-      <c r="F120" s="34"/>
-      <c r="G120" s="35"/>
+      <c r="A120" s="34"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="35"/>
+      <c r="D120" s="35"/>
+      <c r="E120" s="35"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="36"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="33"/>
-      <c r="B121" s="34"/>
-      <c r="C121" s="34"/>
-      <c r="D121" s="34"/>
-      <c r="E121" s="34"/>
-      <c r="F121" s="34"/>
-      <c r="G121" s="35"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="35"/>
+      <c r="F121" s="35"/>
+      <c r="G121" s="36"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="33"/>
-      <c r="B122" s="34"/>
-      <c r="C122" s="34"/>
-      <c r="D122" s="34"/>
-      <c r="E122" s="34"/>
-      <c r="F122" s="34"/>
-      <c r="G122" s="35"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
+      <c r="F122" s="35"/>
+      <c r="G122" s="36"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="33"/>
-      <c r="B123" s="34"/>
-      <c r="C123" s="34"/>
-      <c r="D123" s="34"/>
-      <c r="E123" s="34"/>
-      <c r="F123" s="34"/>
-      <c r="G123" s="35"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="35"/>
+      <c r="F123" s="35"/>
+      <c r="G123" s="36"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="33"/>
-      <c r="B124" s="34"/>
-      <c r="C124" s="34"/>
-      <c r="D124" s="34"/>
-      <c r="E124" s="34"/>
-      <c r="F124" s="34"/>
-      <c r="G124" s="35"/>
+      <c r="A124" s="34"/>
+      <c r="B124" s="35"/>
+      <c r="C124" s="35"/>
+      <c r="D124" s="35"/>
+      <c r="E124" s="35"/>
+      <c r="F124" s="35"/>
+      <c r="G124" s="36"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="33"/>
-      <c r="B125" s="34"/>
-      <c r="C125" s="34"/>
-      <c r="D125" s="34"/>
-      <c r="E125" s="34"/>
-      <c r="F125" s="34"/>
-      <c r="G125" s="35"/>
+      <c r="A125" s="34"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="35"/>
+      <c r="D125" s="35"/>
+      <c r="E125" s="35"/>
+      <c r="F125" s="35"/>
+      <c r="G125" s="36"/>
     </row>
     <row r="126" ht="15.5" customHeight="1">
-      <c r="A126" s="33"/>
-      <c r="B126" s="34"/>
-      <c r="C126" s="34"/>
-      <c r="D126" s="34"/>
-      <c r="E126" s="34"/>
-      <c r="F126" s="34"/>
-      <c r="G126" s="35"/>
+      <c r="A126" s="34"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
+      <c r="D126" s="35"/>
+      <c r="E126" s="35"/>
+      <c r="F126" s="35"/>
+      <c r="G126" s="36"/>
     </row>
     <row r="127" ht="15.5" customHeight="1">
-      <c r="A127" s="36"/>
-      <c r="B127" s="37"/>
-      <c r="C127" s="37"/>
-      <c r="D127" s="37"/>
-      <c r="E127" s="37"/>
-      <c r="F127" s="37"/>
-      <c r="G127" s="38"/>
+      <c r="A127" s="37"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Diary update Duo Chai (#338)
* update diary entry

* update diary

* update diary Duo Chai
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -298,6 +298,36 @@
   </si>
   <si>
     <t>After discussing with my teammates, i know more about this project. Sometimes brainstorming brings you what u ignores before. I am learning towards the way of what a senior would do.</t>
+  </si>
+  <si>
+    <t>Follow the lecture professor</t>
+  </si>
+  <si>
+    <t>Learnt to try to be skeptical, drawing examples and simulating at the same time when reviewing code. Know more about other projects, and others’ dilemmas</t>
+  </si>
+  <si>
+    <t>Learnt more about what an expert would do in reverse engineering. Also after learning this course for 5 weeks, we are gonna have a midterm next week. Will review the knowledges and practice tools that we learnt before in the next few days and prepare for the midterm.</t>
+  </si>
+  <si>
+    <t>Do well in midterm</t>
+  </si>
+  <si>
+    <t>finished midterm!!!! big achievement!!!</t>
+  </si>
+  <si>
+    <t>Midterm is kinda hard to describe, since it has many subjective questions. But it’s also the meaning of this course. There is no certain ways to reverse engineer, what we can do is to be subjective and try our best based on some useful concepts. I hope i did it well. Also about the lecture, it is kinda interesting to think about the big picture of one program. Thinking of it stakeholder, functionality and key developers could let us know more than the program itself, like, the community, and the future.</t>
+  </si>
+  <si>
+    <t>13:00-17:00</t>
+  </si>
+  <si>
+    <t>Finish homework,3 resubmit homework2</t>
+  </si>
+  <si>
+    <t>finished homework2, and resubmit our homework3</t>
+  </si>
+  <si>
+    <t>For our previous homework report, we didn’t realize how the report structure will influence reader’s readability. We change the structure of our homework report and make the content more logical this time.</t>
   </si>
 </sst>
 </file>
@@ -2222,31 +2252,73 @@
       </c>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
+      <c r="A26" s="25">
+        <v>43867</v>
+      </c>
+      <c r="B26" t="s" s="20">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s" s="20">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s" s="27">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s" s="20">
+        <v>92</v>
+      </c>
+      <c r="G26" t="s" s="32">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
+      <c r="A27" s="25">
+        <v>43874</v>
+      </c>
+      <c r="B27" t="s" s="29">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s" s="20">
+        <v>93</v>
+      </c>
+      <c r="E27" t="s" s="20">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s" s="20">
+        <v>95</v>
+      </c>
+      <c r="G27" t="s" s="24">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
+      <c r="A28" s="25">
+        <v>43880</v>
+      </c>
+      <c r="B28" t="s" s="20">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s" s="20">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s" s="20">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s" s="20">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s" s="20">
+        <v>99</v>
+      </c>
+      <c r="G28" t="s" s="24">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" ht="15.5" customHeight="1">
       <c r="A29" s="34"/>

</xml_diff>

<commit_message>
update diary Duo Chai (#405)
* update diary Duo Chai

* update diary Duo Chai
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -328,6 +328,42 @@
   </si>
   <si>
     <t>For our previous homework report, we didn’t realize how the report structure will influence reader’s readability. We change the structure of our homework report and make the content more logical this time.</t>
+  </si>
+  <si>
+    <t>leant to dive deeper within a project from architecture perspective, also social context perspective</t>
+  </si>
+  <si>
+    <t>Instead of doing more research on class level and feature level of a project, we learnt to do more work based on an architectural perspective. This will give us a more concreted sense of the whole program. Also we learnt to know the importance of looking at the social context of a project before deciding to contribute. It might be frustrated if maintainers do not maintain this project any more when you contribute.</t>
+  </si>
+  <si>
+    <t>13:30 - 17:00</t>
+  </si>
+  <si>
+    <t>Soobin</t>
+  </si>
+  <si>
+    <t>finish homework3</t>
+  </si>
+  <si>
+    <t>talked about interesting open issues and PRs, finished social context of our program</t>
+  </si>
+  <si>
+    <t>Some of these PRs are quite ridiculous. Some people they just want to be a contributor by doing minimal, such as fixing typo in commands. And that is all they do. So funny and things also happen in reality.</t>
+  </si>
+  <si>
+    <t>Nervous</t>
+  </si>
+  <si>
+    <t>14:00 - 17:00 &amp; 19:30 - 21:00</t>
+  </si>
+  <si>
+    <t>finished architecture recovering</t>
+  </si>
+  <si>
+    <t>What we did in class by dragging and grouping Pacman classes in UML diagram is kinda a bottom up comprehension. But when it comes to a 100K LOC program, it is impossible to use that strategy since there are SOOOO many classes and interfaces. So we used a top down way to comprehend all the meaningful features first then top down confirm our hypothesis of the architecture by taking a look at these folders’ name, files implementations. It works fine</t>
+  </si>
+  <si>
+    <t>Good, relief</t>
   </si>
 </sst>
 </file>
@@ -2321,31 +2357,73 @@
       </c>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="A29" s="25">
+        <v>43881</v>
+      </c>
+      <c r="B29" t="s" s="20">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s" s="20">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s" s="20">
+        <v>101</v>
+      </c>
+      <c r="G29" t="s" s="24">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="25">
+        <v>43886</v>
+      </c>
+      <c r="B30" t="s" s="20">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s" s="20">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s" s="20">
+        <v>104</v>
+      </c>
+      <c r="E30" t="s" s="20">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s" s="20">
+        <v>106</v>
+      </c>
+      <c r="G30" t="s" s="24">
+        <v>107</v>
+      </c>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
+      <c r="A31" s="25">
+        <v>43887</v>
+      </c>
+      <c r="B31" t="s" s="20">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s" s="20">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s" s="20">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s" s="20">
+        <v>109</v>
+      </c>
+      <c r="F31" t="s" s="20">
+        <v>110</v>
+      </c>
+      <c r="G31" t="s" s="24">
+        <v>111</v>
+      </c>
     </row>
     <row r="32" ht="15.5" customHeight="1">
       <c r="A32" s="34"/>

</xml_diff>

<commit_message>
update diary entry Duo Chai
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -300,9 +300,6 @@
     <t>After discussing with my teammates, i know more about this project. Sometimes brainstorming brings you what u ignores before. I am learning towards the way of what a senior would do.</t>
   </si>
   <si>
-    <t>Follow the lecture professor</t>
-  </si>
-  <si>
     <t>Learnt to try to be skeptical, drawing examples and simulating at the same time when reviewing code. Know more about other projects, and others’ dilemmas</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>Good, relief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learnt more about key expert features, learnt design patterns. </t>
+  </si>
+  <si>
+    <t>Coding is not just about improvising, it’s also about pattern, experience and skill.</t>
   </si>
 </sst>
 </file>
@@ -2298,13 +2301,13 @@
         <v>16</v>
       </c>
       <c r="D26" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s" s="27">
         <v>90</v>
       </c>
-      <c r="E26" t="s" s="27">
+      <c r="F26" t="s" s="20">
         <v>91</v>
-      </c>
-      <c r="F26" t="s" s="20">
-        <v>92</v>
       </c>
       <c r="G26" t="s" s="32">
         <v>53</v>
@@ -2321,13 +2324,13 @@
         <v>16</v>
       </c>
       <c r="D27" t="s" s="20">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s" s="20">
         <v>93</v>
       </c>
-      <c r="E27" t="s" s="20">
+      <c r="F27" t="s" s="20">
         <v>94</v>
-      </c>
-      <c r="F27" t="s" s="20">
-        <v>95</v>
       </c>
       <c r="G27" t="s" s="24">
         <v>20</v>
@@ -2338,19 +2341,19 @@
         <v>43880</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s" s="20">
         <v>34</v>
       </c>
       <c r="D28" t="s" s="20">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s" s="20">
         <v>97</v>
       </c>
-      <c r="E28" t="s" s="20">
+      <c r="F28" t="s" s="20">
         <v>98</v>
-      </c>
-      <c r="F28" t="s" s="20">
-        <v>99</v>
       </c>
       <c r="G28" t="s" s="24">
         <v>53</v>
@@ -2370,10 +2373,10 @@
         <v>63</v>
       </c>
       <c r="E29" t="s" s="20">
+        <v>99</v>
+      </c>
+      <c r="F29" t="s" s="20">
         <v>100</v>
-      </c>
-      <c r="F29" t="s" s="20">
-        <v>101</v>
       </c>
       <c r="G29" t="s" s="24">
         <v>53</v>
@@ -2384,22 +2387,22 @@
         <v>43886</v>
       </c>
       <c r="B30" t="s" s="20">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s" s="20">
         <v>102</v>
       </c>
-      <c r="C30" t="s" s="20">
+      <c r="D30" t="s" s="20">
         <v>103</v>
       </c>
-      <c r="D30" t="s" s="20">
+      <c r="E30" t="s" s="20">
         <v>104</v>
       </c>
-      <c r="E30" t="s" s="20">
+      <c r="F30" t="s" s="20">
         <v>105</v>
       </c>
-      <c r="F30" t="s" s="20">
+      <c r="G30" t="s" s="24">
         <v>106</v>
-      </c>
-      <c r="G30" t="s" s="24">
-        <v>107</v>
       </c>
     </row>
     <row r="31" ht="15.5" customHeight="1">
@@ -2407,32 +2410,46 @@
         <v>43887</v>
       </c>
       <c r="B31" t="s" s="20">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s" s="20">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s" s="20">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s" s="20">
         <v>108</v>
       </c>
-      <c r="C31" t="s" s="20">
-        <v>103</v>
-      </c>
-      <c r="D31" t="s" s="20">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s" s="20">
+      <c r="F31" t="s" s="20">
         <v>109</v>
       </c>
-      <c r="F31" t="s" s="20">
+      <c r="G31" t="s" s="24">
         <v>110</v>
       </c>
-      <c r="G31" t="s" s="24">
+    </row>
+    <row r="32" ht="15.5" customHeight="1">
+      <c r="A32" s="25">
+        <v>43888</v>
+      </c>
+      <c r="B32" t="s" s="20">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s" s="20">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
+      <c r="F32" t="s" s="20">
+        <v>112</v>
+      </c>
+      <c r="G32" t="s" s="24">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" ht="15.5" customHeight="1">
       <c r="A33" s="34"/>

</xml_diff>

<commit_message>
Update Diary Entry Duo Chai (#434)
* update diary Duo Chai

* update diary Duo Chai

* update diary entry Duo Chai
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -300,9 +300,6 @@
     <t>After discussing with my teammates, i know more about this project. Sometimes brainstorming brings you what u ignores before. I am learning towards the way of what a senior would do.</t>
   </si>
   <si>
-    <t>Follow the lecture professor</t>
-  </si>
-  <si>
     <t>Learnt to try to be skeptical, drawing examples and simulating at the same time when reviewing code. Know more about other projects, and others’ dilemmas</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>Good, relief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learnt more about key expert features, learnt design patterns. </t>
+  </si>
+  <si>
+    <t>Coding is not just about improvising, it’s also about pattern, experience and skill.</t>
   </si>
 </sst>
 </file>
@@ -2298,13 +2301,13 @@
         <v>16</v>
       </c>
       <c r="D26" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s" s="27">
         <v>90</v>
       </c>
-      <c r="E26" t="s" s="27">
+      <c r="F26" t="s" s="20">
         <v>91</v>
-      </c>
-      <c r="F26" t="s" s="20">
-        <v>92</v>
       </c>
       <c r="G26" t="s" s="32">
         <v>53</v>
@@ -2321,13 +2324,13 @@
         <v>16</v>
       </c>
       <c r="D27" t="s" s="20">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s" s="20">
         <v>93</v>
       </c>
-      <c r="E27" t="s" s="20">
+      <c r="F27" t="s" s="20">
         <v>94</v>
-      </c>
-      <c r="F27" t="s" s="20">
-        <v>95</v>
       </c>
       <c r="G27" t="s" s="24">
         <v>20</v>
@@ -2338,19 +2341,19 @@
         <v>43880</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s" s="20">
         <v>34</v>
       </c>
       <c r="D28" t="s" s="20">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s" s="20">
         <v>97</v>
       </c>
-      <c r="E28" t="s" s="20">
+      <c r="F28" t="s" s="20">
         <v>98</v>
-      </c>
-      <c r="F28" t="s" s="20">
-        <v>99</v>
       </c>
       <c r="G28" t="s" s="24">
         <v>53</v>
@@ -2370,10 +2373,10 @@
         <v>63</v>
       </c>
       <c r="E29" t="s" s="20">
+        <v>99</v>
+      </c>
+      <c r="F29" t="s" s="20">
         <v>100</v>
-      </c>
-      <c r="F29" t="s" s="20">
-        <v>101</v>
       </c>
       <c r="G29" t="s" s="24">
         <v>53</v>
@@ -2384,22 +2387,22 @@
         <v>43886</v>
       </c>
       <c r="B30" t="s" s="20">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s" s="20">
         <v>102</v>
       </c>
-      <c r="C30" t="s" s="20">
+      <c r="D30" t="s" s="20">
         <v>103</v>
       </c>
-      <c r="D30" t="s" s="20">
+      <c r="E30" t="s" s="20">
         <v>104</v>
       </c>
-      <c r="E30" t="s" s="20">
+      <c r="F30" t="s" s="20">
         <v>105</v>
       </c>
-      <c r="F30" t="s" s="20">
+      <c r="G30" t="s" s="24">
         <v>106</v>
-      </c>
-      <c r="G30" t="s" s="24">
-        <v>107</v>
       </c>
     </row>
     <row r="31" ht="15.5" customHeight="1">
@@ -2407,32 +2410,46 @@
         <v>43887</v>
       </c>
       <c r="B31" t="s" s="20">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s" s="20">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s" s="20">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s" s="20">
         <v>108</v>
       </c>
-      <c r="C31" t="s" s="20">
-        <v>103</v>
-      </c>
-      <c r="D31" t="s" s="20">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s" s="20">
+      <c r="F31" t="s" s="20">
         <v>109</v>
       </c>
-      <c r="F31" t="s" s="20">
+      <c r="G31" t="s" s="24">
         <v>110</v>
       </c>
-      <c r="G31" t="s" s="24">
+    </row>
+    <row r="32" ht="15.5" customHeight="1">
+      <c r="A32" s="25">
+        <v>43888</v>
+      </c>
+      <c r="B32" t="s" s="20">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s" s="20">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
+      <c r="F32" t="s" s="20">
+        <v>112</v>
+      </c>
+      <c r="G32" t="s" s="24">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" ht="15.5" customHeight="1">
       <c r="A33" s="34"/>

</xml_diff>

<commit_message>
fix typo in diary
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -357,7 +357,7 @@
     <t>finished architecture recovering</t>
   </si>
   <si>
-    <t>What we did in class by dragging and grouping Pacman classes in UML diagram is kinda a bottom up comprehension. But when it comes to a 100K LOC program, it is impossible to use that strategy since there are SOOOO many classes and interfaces. So we used a top down way to comprehend all the meaningful features first then top down confirm our hypothesis of the architecture by taking a look at these folders’ name, files implementations. It works fine</t>
+    <t>What we did in class by dragging and grouping Pacman classes in UML diagram is kind of a bottom up comprehension. But when it comes to a 100K LOC program, it is impossible to use that strategy since there are SOOOO many classes and interfaces. So we used a top down way to comprehend all the meaningful features first then top down confirm our hypothesis of the architecture by taking a look at these folders’ name, files implementations. It works fine</t>
   </si>
   <si>
     <t>Good, relief</t>
@@ -366,7 +366,7 @@
     <t xml:space="preserve">Learnt more about key expert features, learnt design patterns. </t>
   </si>
   <si>
-    <t>Coding is not just about improvising, it’s also about pattern, experience and skill.</t>
+    <t>Coding is not just about improvising, it’s also about pattern, experience and skill. Pattern helps reflecting mental models which is useful in software understanding and reverse engineering</t>
   </si>
   <si>
     <t>20:45-21:20</t>

</xml_diff>